<commit_message>
thêm dữ liệu bằng excel
</commit_message>
<xml_diff>
--- a/public/insert_template/themlk.xlsx
+++ b/public/insert_template/themlk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\PHP\quanlycuahang\public\insert_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00CFC67-C659-4034-98A7-7F85070CEAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C9A209-AD38-4B56-9B0C-B591EADF7BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5868" yWindow="564" windowWidth="17172" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thêm linh kiện" sheetId="1" r:id="rId1"/>
@@ -51,10 +51,6 @@
     <t>Giá bán</t>
   </si>
   <si>
-    <t>Trạng thái
-(Mã trạng thái)</t>
-  </si>
-  <si>
     <t>Thông tin khác
 (TK?TT*TK?TT)</t>
   </si>
@@ -66,12 +62,6 @@
     <t>(Ví dụ)</t>
   </si>
   <si>
-    <t>Mã linh kiện</t>
-  </si>
-  <si>
-    <t>Tên linh kiện</t>
-  </si>
-  <si>
     <t>Chỉ số</t>
   </si>
   <si>
@@ -94,13 +84,69 @@
   </si>
   <si>
     <t>Chỉ số?2UF</t>
+  </si>
+  <si>
+    <r>
+      <t>Trạng thái(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+(Mã trạng thái)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mã linh kiện(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tên linh kiện(*)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +158,14 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -436,15 +490,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.3984375" customWidth="1"/>
     <col min="4" max="4" width="16.69921875" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" customWidth="1"/>
@@ -489,16 +543,16 @@
     </row>
     <row r="3" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -510,30 +564,30 @@
         <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -551,13 +605,13 @@
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>